<commit_message>
create auth & authoriz
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="110">
   <si>
     <t>HTTP method</t>
   </si>
@@ -193,27 +193,15 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Set up the project repository (Git).</t>
-  </si>
-  <si>
-    <t>Create the basic folder structure for the frontend (React) and backend (Node.js/Express).</t>
-  </si>
-  <si>
     <t>Initialize the database schema (MongoDB):</t>
   </si>
   <si>
-    <t>Define Role, User, Project, Ticket, Card, and Activity schemas.</t>
-  </si>
-  <si>
     <t>Set up REST API routes for User and Role schemas.</t>
   </si>
   <si>
     <t>Test User and Role API routes using Postman or Insomnia.</t>
   </si>
   <si>
-    <t>Day 2</t>
-  </si>
-  <si>
     <t>Implement user registration and login functionality in the frontend.</t>
   </si>
   <si>
@@ -229,12 +217,6 @@
     <t>Set up role-based access control for admin features.</t>
   </si>
   <si>
-    <t>Test user registration, login, and role management functionalities.</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
     <t>Set up API routes for Project and Ticket schemas in the backend.</t>
   </si>
   <si>
@@ -244,51 +226,24 @@
     <t>Connect the frontend to the backend for project and ticket management.</t>
   </si>
   <si>
-    <t>Test functionality for adding, updating, and deleting projects and tickets.</t>
-  </si>
-  <si>
-    <t>Create pages for About and Contact Us.</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
     <t>Set up API routes for Card and Activity schemas in the backend.</t>
   </si>
   <si>
     <t>Implement frontend for creating and managing cards (subtasks) within tickets.</t>
   </si>
   <si>
-    <t>Connect frontend to backend for card and activity management.</t>
-  </si>
-  <si>
     <t>Implement logging activities (comments, status changes) for cards.</t>
   </si>
   <si>
-    <t>Test the entire flow from creating a ticket to adding cards and logging activities.</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
     <t>Implement notification feature in the backend (endpoints for sending and retrieving notifications).</t>
   </si>
   <si>
     <t>Integrate a drag-and-drop library (e.g., React Beautiful DnD) for cards and tickets.</t>
   </si>
   <si>
-    <t>Implement the notification display in the frontend.</t>
-  </si>
-  <si>
-    <t>Add light-dark mode toggle feature in the frontend.</t>
-  </si>
-  <si>
     <t>Implement favorite project functionality (mark/unmark projects as favorites).</t>
   </si>
   <si>
-    <t>Day 6</t>
-  </si>
-  <si>
     <t>Perform end-to-end testing of all functionalities.</t>
   </si>
   <si>
@@ -329,6 +284,79 @@
   </si>
   <si>
     <t>/board</t>
+  </si>
+  <si>
+    <t>Create the basic folder structure for the backend (Node.js/Express).</t>
+  </si>
+  <si>
+    <t>Define schemas: Role, User, Project, Ticket, Card, and Activity.</t>
+  </si>
+  <si>
+    <t>set up the project repository (Git).</t>
+  </si>
+  <si>
+    <t>Project &amp; Ticket APIs</t>
+  </si>
+  <si>
+    <t>Initial Setup and Database Schema</t>
+  </si>
+  <si>
+    <t>REST API &amp; User Management</t>
+  </si>
+  <si>
+    <t>User Management Frontend</t>
+  </si>
+  <si>
+    <t>Create the basic folder structure for the frontend (React).</t>
+  </si>
+  <si>
+    <t>Project, Ticket, and Card Management</t>
+  </si>
+  <si>
+    <t>UI Enhancements &amp; Testing</t>
+  </si>
+  <si>
+    <t>Implement notification display in the frontend.</t>
+  </si>
+  <si>
+    <t>Add a light-dark mode toggle feature in the frontend.</t>
+  </si>
+  <si>
+    <t>Extra tasks or polish (as needed)</t>
+  </si>
+  <si>
+    <t>Day 2
+6-10-2024</t>
+  </si>
+  <si>
+    <t>Day 3
+7-10-2024</t>
+  </si>
+  <si>
+    <t>Day 4
+8-10-2024</t>
+  </si>
+  <si>
+    <t>check backend</t>
+  </si>
+  <si>
+    <t>Day 5
+9-10-2024</t>
+  </si>
+  <si>
+    <t>Day 6
+10-10-2024</t>
+  </si>
+  <si>
+    <t>Day 7
+11-10-2024</t>
+  </si>
+  <si>
+    <t>check All Project</t>
+  </si>
+  <si>
+    <t>Day 8
+12-10-2024</t>
   </si>
 </sst>
 </file>
@@ -375,7 +403,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,12 +430,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -430,11 +470,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -442,20 +519,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -463,8 +528,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -472,17 +537,46 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -788,20 +882,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -854,20 +948,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -982,20 +1076,20 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1020,7 +1114,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1044,20 +1138,20 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1170,20 +1264,20 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1300,20 +1394,20 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,20 +1524,20 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1551,411 +1645,394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="2" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C1" s="8"/>
+      <c r="C1" s="15" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="18">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="18">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="10">
+    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="18">
+        <v>4</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="10">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="10">
+      <c r="C9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="10">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="10">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="10">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="10">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="10">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="10">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="10">
+      <c r="C25" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="10">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="10">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="10">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="10">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="10">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="10">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="10">
-        <v>6</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="C38" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="10">
         <v>1</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="10">
+      <c r="C40" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="17">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="10">
+      <c r="C45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
+      <c r="B46" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="10">
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="14"/>
+      <c r="B47" s="17">
         <v>4</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="10">
-        <v>5</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="10">
-        <v>6</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="10">
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="25">
         <v>1</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="10">
+      <c r="C48" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="26"/>
+      <c r="C49" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="27"/>
+      <c r="C50" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="25">
         <v>2</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="10">
-        <v>3</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="10">
-        <v>4</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="10">
-        <v>5</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="10">
-        <v>1</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="10">
-        <v>2</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="10">
-        <v>3</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="10">
-        <v>4</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="10">
-        <v>5</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="10">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="C51" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
-      <c r="B33" s="10">
-        <v>2</v>
-      </c>
-      <c r="C33" s="11" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="26"/>
+      <c r="C52" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
-      <c r="B34" s="10">
-        <v>3</v>
-      </c>
-      <c r="C34" s="11" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="27"/>
+      <c r="C53" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="10">
-        <v>4</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
-      <c r="B36" s="10">
-        <v>5</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="10">
-        <v>1</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="10">
-        <v>2</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
-      <c r="B41" s="10">
-        <v>3</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
-      <c r="B42" s="10">
-        <v>4</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="10">
-        <v>5</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="17">
-        <v>1</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="17">
-        <v>2</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="8"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="8"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A44:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create add ticket and get all ticket fun
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -606,6 +606,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,7 +637,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,20 +941,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1007,20 +1007,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1185,48 +1185,48 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="16" t="s">
         <v>126</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="16" t="s">
         <v>127</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="16" t="s">
         <v>128</v>
       </c>
       <c r="F24" s="1"/>
@@ -1313,20 +1313,20 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1375,20 +1375,20 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1460,7 +1460,7 @@
         <v>19</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
         <v>50</v>
@@ -1476,7 +1476,7 @@
         <v>19</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
         <v>51</v>
@@ -1501,20 +1501,20 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1631,20 +1631,20 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,20 +1761,20 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="11">
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="11">
         <v>2</v>
       </c>
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="11">
         <v>3</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="11">
         <v>4</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B8" s="8">
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="8">
         <v>2</v>
       </c>
@@ -1965,7 +1965,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="8">
         <v>3</v>
       </c>
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="8">
         <v>4</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B14" s="8">
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="8">
         <v>2</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="8">
         <v>3</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="25" t="s">
         <v>101</v>
       </c>
       <c r="B22" s="8">
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="8">
         <v>2</v>
       </c>
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="8">
         <v>3</v>
       </c>
@@ -2062,7 +2062,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="8">
         <v>4</v>
       </c>
@@ -2076,7 +2076,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="25" t="s">
         <v>102</v>
       </c>
       <c r="B28" s="8">
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="8">
         <v>2</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="8">
         <v>3</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="8">
         <v>4</v>
       </c>
@@ -2119,7 +2119,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="8">
@@ -2130,7 +2130,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="8">
         <v>2</v>
       </c>
@@ -2139,7 +2139,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="8">
         <v>3</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="8">
         <v>4</v>
       </c>
@@ -2157,7 +2157,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="8">
         <v>5</v>
       </c>
@@ -2182,7 +2182,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B44" s="10">
@@ -2193,7 +2193,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="10">
         <v>2</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="10">
         <v>3</v>
       </c>
@@ -2211,7 +2211,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="21"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="10">
         <v>4</v>
       </c>
@@ -2220,7 +2220,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="17">
+      <c r="B48" s="18">
         <v>1</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -2228,19 +2228,19 @@
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
+      <c r="B49" s="19"/>
       <c r="C49" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="19"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="17">
+      <c r="B51" s="18">
         <v>2</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -2248,13 +2248,13 @@
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="18"/>
+      <c r="B52" s="19"/>
       <c r="C52" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="6" t="s">
         <v>81</v>
       </c>

</xml_diff>